<commit_message>
Updates to Sine plotting and subject info parameter changes
</commit_message>
<xml_diff>
--- a/SubjectInfo.xlsx
+++ b/SubjectInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andriannaayiotis/Documents/MATLAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andriannaayiotis/Documents/MATLAB/VOGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F02F0C4-A3C7-A142-AABF-1A3F03374FF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57364985-6F88-5C40-B2EF-2CF20AD83E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
+    <workbookView xWindow="-15800" yWindow="-5000" windowWidth="15500" windowHeight="8860" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C117F-76BB-5A4B-A691-C2F0544A3D8B}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -450,7 +450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -472,8 +472,14 @@
       <c r="G2" s="1">
         <v>43960</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>44195</v>
+      </c>
+      <c r="I2" s="1">
+        <v>44237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -489,8 +495,20 @@
       <c r="E3" s="1">
         <v>42746</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3" s="1">
+        <v>43924</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43950</v>
+      </c>
+      <c r="H3" s="1">
+        <v>43982</v>
+      </c>
+      <c r="I3" s="1">
+        <v>44284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -507,10 +525,10 @@
         <v>43551</v>
       </c>
       <c r="F4" s="1">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -529,8 +547,11 @@
       <c r="F5" s="1">
         <v>43925</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -546,8 +567,11 @@
       <c r="E6" s="1">
         <v>43928</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>44249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -563,8 +587,11 @@
       <c r="E7" s="1">
         <v>44064</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <v>43942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -578,13 +605,11 @@
         <v>43648</v>
       </c>
       <c r="E8" s="1">
-        <v>43954</v>
-      </c>
-      <c r="F8" s="1">
-        <v>44037</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44312</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -609,8 +634,11 @@
       <c r="H9" s="1">
         <v>43996</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>44300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -625,6 +653,12 @@
       </c>
       <c r="E10" s="1">
         <v>44138</v>
+      </c>
+      <c r="F10" s="1">
+        <v>44252</v>
+      </c>
+      <c r="G10" s="1">
+        <v>44278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MVI010, small updates to plot figures and fixed timestamp error with MakeNotes
</commit_message>
<xml_diff>
--- a/SubjectInfo.xlsx
+++ b/SubjectInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andriannaayiotis/Documents/MATLAB/VOGA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57364985-6F88-5C40-B2EF-2CF20AD83E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78EBD39-767A-BB4A-B0A6-1ACC266DA967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15800" yWindow="-5000" windowWidth="15500" windowHeight="8860" xr2:uid="{5492E525-EE99-8040-A434-353228F4B206}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>MVI001R019</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Settings Changes</t>
+  </si>
+  <si>
+    <t>MVI010R141</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F4C117F-76BB-5A4B-A691-C2F0544A3D8B}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,6 +664,17 @@
         <v>44278</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44433</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>